<commit_message>
Data Accumulated and Labelled for Sites 1:40 and aggregated into one dataset
</commit_message>
<xml_diff>
--- a/Second Iteration Data/data_gathered_part_first_segmentation_1.xlsx
+++ b/Second Iteration Data/data_gathered_part_first_segmentation_1.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Passion\Machine Learning\Projects\Semantic_Web_Parser\Second Iteration Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398712CE-4504-4279-9F33-83E4F739D2D6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="684" yWindow="1176" windowWidth="9600" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>tag_h</t>
   </si>
@@ -72,28 +77,40 @@
   </si>
   <si>
     <t>nan</t>
+  </si>
+  <si>
+    <t>label</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -108,26 +125,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -415,20 +450,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:P4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -474,30 +505,33 @@
       <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="Q1" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>48</v>
       </c>
-      <c r="G2" t="n">
-        <v>0.03414634146341464</v>
-      </c>
-      <c r="H2" t="n">
+      <c r="G2">
+        <v>3.4146341463414637E-2</v>
+      </c>
+      <c r="H2">
         <v>0</v>
       </c>
       <c r="I2" t="s">
@@ -506,48 +540,51 @@
       <c r="J2" t="s">
         <v>15</v>
       </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" t="n">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>10</v>
       </c>
-      <c r="M2" t="n">
+      <c r="M2">
         <v>130</v>
       </c>
-      <c r="N2" t="n">
+      <c r="N2">
         <v>1266.400024414062</v>
       </c>
-      <c r="O2" t="n">
-        <v>0.02257101149312446</v>
+      <c r="O2">
+        <v>2.257101149312446E-2</v>
       </c>
       <c r="P2" t="s">
         <v>16</v>
       </c>
+      <c r="Q2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>12</v>
       </c>
-      <c r="C3" t="n">
+      <c r="C3">
         <v>45</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>45</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" t="n">
+      <c r="F3">
         <v>3193</v>
       </c>
-      <c r="G3" t="n">
-        <v>0.0009322922736277824</v>
-      </c>
-      <c r="H3" t="n">
+      <c r="G3">
+        <v>9.3229227362778236E-4</v>
+      </c>
+      <c r="H3">
         <v>0</v>
       </c>
       <c r="I3" t="s">
@@ -556,48 +593,51 @@
       <c r="J3" t="s">
         <v>15</v>
       </c>
-      <c r="K3" t="n">
+      <c r="K3">
         <v>166</v>
       </c>
-      <c r="L3" t="n">
+      <c r="L3">
         <v>140</v>
       </c>
-      <c r="M3" t="n">
+      <c r="M3">
         <v>5594.60009765625</v>
       </c>
-      <c r="N3" t="n">
+      <c r="N3">
         <v>934</v>
       </c>
-      <c r="O3" t="n">
-        <v>0.7163952278115996</v>
+      <c r="O3">
+        <v>0.71639522781159959</v>
       </c>
       <c r="P3" t="s">
         <v>17</v>
       </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" t="n">
+      <c r="F4">
         <v>1</v>
       </c>
       <c r="G4" t="s">
         <v>18</v>
       </c>
-      <c r="H4" t="n">
+      <c r="H4">
         <v>0</v>
       </c>
       <c r="I4" t="s">
@@ -606,26 +646,30 @@
       <c r="J4" t="s">
         <v>15</v>
       </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>0</v>
       </c>
       <c r="P4" t="s">
         <v>18</v>
       </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>